<commit_message>
Added x values to the thermocouple temperature readings
</commit_message>
<xml_diff>
--- a/Forced Convection/Formatted Test Data.xlsx
+++ b/Forced Convection/Formatted Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rutgersconnect-my.sharepoint.com/personal/brk70_scarletmail_rutgers_edu/Documents/Senior Year/Senior Spring/ME Lab II/Forced Convection Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1b26bea70f0b/Personal/GitHub/School-Programs/Forced Convection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{335CF15A-9485-4D47-A487-6EB69C949C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55D8298F-D410-46FF-A014-7610D462D7F3}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{335CF15A-9485-4D47-A487-6EB69C949C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FAC34B5-2DD9-41C9-91F4-1C0F3A95C4A5}"/>
   <bookViews>
-    <workbookView xWindow="-3744" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{CE436325-4879-4D4B-B168-3D4926EFFFD0}"/>
+    <workbookView xWindow="14160" yWindow="-21600" windowWidth="19410" windowHeight="20985" firstSheet="2" activeTab="3" xr2:uid="{CE436325-4879-4D4B-B168-3D4926EFFFD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1 - High MFR Low Crnt " sheetId="1" r:id="rId1"/>
@@ -449,9 +449,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21114F00-AC07-4D56-B2A2-E22DD7B79111}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>45.833848476000014</v>
+      </c>
+      <c r="B2">
+        <v>53.320685295999986</v>
+      </c>
+      <c r="C2">
+        <v>47.663612560000033</v>
+      </c>
+      <c r="D2">
+        <v>47.883861887999998</v>
+      </c>
+      <c r="E2">
+        <v>48.317890712000008</v>
+      </c>
+      <c r="F2">
+        <v>48.838252708000013</v>
+      </c>
+      <c r="G2">
+        <v>48.692147628000015</v>
+      </c>
+      <c r="H2">
+        <v>59.082457548000022</v>
+      </c>
+      <c r="I2">
+        <v>27.904625571999993</v>
+      </c>
+      <c r="J2">
+        <v>56.781315444000008</v>
+      </c>
+      <c r="K2">
+        <v>27.570950496000016</v>
+      </c>
+      <c r="L2">
+        <v>57.109659087999958</v>
+      </c>
+      <c r="M2">
+        <v>27.854072176000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12.5</v>
+      </c>
+      <c r="B3">
+        <v>28.125</v>
+      </c>
+      <c r="C3">
+        <v>40.5</v>
+      </c>
+      <c r="D3">
+        <v>47.125</v>
+      </c>
+      <c r="E3">
+        <v>53.75</v>
+      </c>
+      <c r="F3">
+        <v>60.375</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>37</v>
+      </c>
+      <c r="K3">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>52</v>
+      </c>
+      <c r="M3">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39839E2D-6A79-4CB5-8A3E-B833C43F470E}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="A3:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>56.401438128000024</v>
+      </c>
+      <c r="B2">
+        <v>74.85780509199995</v>
+      </c>
+      <c r="C2">
+        <v>60.717994547999972</v>
+      </c>
+      <c r="D2">
+        <v>61.252896547999988</v>
+      </c>
+      <c r="E2">
+        <v>62.407663280000016</v>
+      </c>
+      <c r="F2">
+        <v>63.871331232000038</v>
+      </c>
+      <c r="G2">
+        <v>63.496727484000012</v>
+      </c>
+      <c r="H2">
+        <v>89.385546439999928</v>
+      </c>
+      <c r="I2">
+        <v>29.662321604000013</v>
+      </c>
+      <c r="J2">
+        <v>83.734234176000001</v>
+      </c>
+      <c r="K2">
+        <v>29.065856199999992</v>
+      </c>
+      <c r="L2">
+        <v>84.183248267999943</v>
+      </c>
+      <c r="M2">
+        <v>29.390111732000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12.5</v>
+      </c>
+      <c r="B3">
+        <v>28.125</v>
+      </c>
+      <c r="C3">
+        <v>40.5</v>
+      </c>
+      <c r="D3">
+        <v>47.125</v>
+      </c>
+      <c r="E3">
+        <v>53.75</v>
+      </c>
+      <c r="F3">
+        <v>60.375</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>37</v>
+      </c>
+      <c r="K3">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>52</v>
+      </c>
+      <c r="M3">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689AE204-CCFC-4B1C-BECA-B5D2A3947A1B}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>62.577041163999965</v>
+      </c>
+      <c r="B2">
+        <v>81.200373528000071</v>
+      </c>
+      <c r="C2">
+        <v>68.339215668000008</v>
+      </c>
+      <c r="D2">
+        <v>69.080182151999963</v>
+      </c>
+      <c r="E2">
+        <v>70.601206687999991</v>
+      </c>
+      <c r="F2">
+        <v>72.508484520000025</v>
+      </c>
+      <c r="G2">
+        <v>71.494419379999997</v>
+      </c>
+      <c r="H2">
+        <v>94.536057184000029</v>
+      </c>
+      <c r="I2">
+        <v>31.47899017999999</v>
+      </c>
+      <c r="J2">
+        <v>91.138442103999964</v>
+      </c>
+      <c r="K2">
+        <v>30.568390367999996</v>
+      </c>
+      <c r="L2">
+        <v>91.453875064000044</v>
+      </c>
+      <c r="M2">
+        <v>31.010239367999983</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12.5</v>
+      </c>
+      <c r="B3">
+        <v>28.125</v>
+      </c>
+      <c r="C3">
+        <v>40.5</v>
+      </c>
+      <c r="D3">
+        <v>47.125</v>
+      </c>
+      <c r="E3">
+        <v>53.75</v>
+      </c>
+      <c r="F3">
+        <v>60.375</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>37</v>
+      </c>
+      <c r="K3">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>52</v>
+      </c>
+      <c r="M3">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8E3B4F-BAA0-4DA9-9879-36A731D2513A}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -504,309 +930,6 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>45.833848476000014</v>
-      </c>
-      <c r="B2">
-        <v>53.320685295999986</v>
-      </c>
-      <c r="C2">
-        <v>47.663612560000033</v>
-      </c>
-      <c r="D2">
-        <v>47.883861887999998</v>
-      </c>
-      <c r="E2">
-        <v>48.317890712000008</v>
-      </c>
-      <c r="F2">
-        <v>48.838252708000013</v>
-      </c>
-      <c r="G2">
-        <v>48.692147628000015</v>
-      </c>
-      <c r="H2">
-        <v>59.082457548000022</v>
-      </c>
-      <c r="I2">
-        <v>27.904625571999993</v>
-      </c>
-      <c r="J2">
-        <v>56.781315444000008</v>
-      </c>
-      <c r="K2">
-        <v>27.570950496000016</v>
-      </c>
-      <c r="L2">
-        <v>57.109659087999958</v>
-      </c>
-      <c r="M2">
-        <v>27.854072176000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39839E2D-6A79-4CB5-8A3E-B833C43F470E}">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>56.401438128000024</v>
-      </c>
-      <c r="B2">
-        <v>74.85780509199995</v>
-      </c>
-      <c r="C2">
-        <v>60.717994547999972</v>
-      </c>
-      <c r="D2">
-        <v>61.252896547999988</v>
-      </c>
-      <c r="E2">
-        <v>62.407663280000016</v>
-      </c>
-      <c r="F2">
-        <v>63.871331232000038</v>
-      </c>
-      <c r="G2">
-        <v>63.496727484000012</v>
-      </c>
-      <c r="H2">
-        <v>89.385546439999928</v>
-      </c>
-      <c r="I2">
-        <v>29.662321604000013</v>
-      </c>
-      <c r="J2">
-        <v>83.734234176000001</v>
-      </c>
-      <c r="K2">
-        <v>29.065856199999992</v>
-      </c>
-      <c r="L2">
-        <v>84.183248267999943</v>
-      </c>
-      <c r="M2">
-        <v>29.390111732000008</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689AE204-CCFC-4B1C-BECA-B5D2A3947A1B}">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>62.577041163999965</v>
-      </c>
-      <c r="B2">
-        <v>81.200373528000071</v>
-      </c>
-      <c r="C2">
-        <v>68.339215668000008</v>
-      </c>
-      <c r="D2">
-        <v>69.080182151999963</v>
-      </c>
-      <c r="E2">
-        <v>70.601206687999991</v>
-      </c>
-      <c r="F2">
-        <v>72.508484520000025</v>
-      </c>
-      <c r="G2">
-        <v>71.494419379999997</v>
-      </c>
-      <c r="H2">
-        <v>94.536057184000029</v>
-      </c>
-      <c r="I2">
-        <v>31.47899017999999</v>
-      </c>
-      <c r="J2">
-        <v>91.138442103999964</v>
-      </c>
-      <c r="K2">
-        <v>30.568390367999996</v>
-      </c>
-      <c r="L2">
-        <v>91.453875064000044</v>
-      </c>
-      <c r="M2">
-        <v>31.010239367999983</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8E3B4F-BAA0-4DA9-9879-36A731D2513A}">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
         <v>51.522925684000022</v>
       </c>
       <c r="B2">
@@ -844,6 +967,47 @@
       </c>
       <c r="M2">
         <v>32.044188036000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12.5</v>
+      </c>
+      <c r="B3">
+        <v>28.125</v>
+      </c>
+      <c r="C3">
+        <v>40.5</v>
+      </c>
+      <c r="D3">
+        <v>47.125</v>
+      </c>
+      <c r="E3">
+        <v>53.75</v>
+      </c>
+      <c r="F3">
+        <v>60.375</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>37</v>
+      </c>
+      <c r="K3">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>52</v>
+      </c>
+      <c r="M3">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split the temperature data by thermocouple group
</commit_message>
<xml_diff>
--- a/Forced Convection/Formatted Test Data.xlsx
+++ b/Forced Convection/Formatted Test Data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="31" documentId="8_{335CF15A-9485-4D47-A487-6EB69C949C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FAC34B5-2DD9-41C9-91F4-1C0F3A95C4A5}"/>
   <bookViews>
-    <workbookView xWindow="-2484" yWindow="-16128" windowWidth="23040" windowHeight="12120" xr2:uid="{CE436325-4879-4D4B-B168-3D4926EFFFD0}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="3" xr2:uid="{CE436325-4879-4D4B-B168-3D4926EFFFD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1 - High MFR Low Crnt " sheetId="1" r:id="rId1"/>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21114F00-AC07-4D56-B2A2-E22DD7B79111}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8E3B4F-BAA0-4DA9-9879-36A731D2513A}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Converted position values to meters in Formatted Data.xlsx
</commit_message>
<xml_diff>
--- a/Forced Convection/Formatted Test Data.xlsx
+++ b/Forced Convection/Formatted Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1b26bea70f0b/Personal/GitHub/School-Programs/Forced Convection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{335CF15A-9485-4D47-A487-6EB69C949C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FAC34B5-2DD9-41C9-91F4-1C0F3A95C4A5}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{335CF15A-9485-4D47-A487-6EB69C949C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDEDD7CF-422C-4B4E-BC6E-8F1CED18822A}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="3" xr2:uid="{CE436325-4879-4D4B-B168-3D4926EFFFD0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE436325-4879-4D4B-B168-3D4926EFFFD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1 - High MFR Low Crnt " sheetId="1" r:id="rId1"/>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21114F00-AC07-4D56-B2A2-E22DD7B79111}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,25 +545,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>12.5</v>
+        <v>0.3175</v>
       </c>
       <c r="B3">
-        <v>28.125</v>
+        <v>0.71437499999999998</v>
       </c>
       <c r="C3">
-        <v>40.5</v>
+        <v>1.0286999999999999</v>
       </c>
       <c r="D3">
-        <v>47.125</v>
+        <v>1.1969749999999999</v>
       </c>
       <c r="E3">
-        <v>53.75</v>
+        <v>1.3652499999999999</v>
       </c>
       <c r="F3">
-        <v>60.375</v>
+        <v>1.533525</v>
       </c>
       <c r="G3">
-        <v>67</v>
+        <v>1.7018</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -572,16 +572,16 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="K3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="L3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
       <c r="M3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
     </row>
   </sheetData>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39839E2D-6A79-4CB5-8A3E-B833C43F470E}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="A3:M3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,25 +687,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>12.5</v>
+        <v>0.3175</v>
       </c>
       <c r="B3">
-        <v>28.125</v>
+        <v>0.71437499999999998</v>
       </c>
       <c r="C3">
-        <v>40.5</v>
+        <v>1.0286999999999999</v>
       </c>
       <c r="D3">
-        <v>47.125</v>
+        <v>1.1969749999999999</v>
       </c>
       <c r="E3">
-        <v>53.75</v>
+        <v>1.3652499999999999</v>
       </c>
       <c r="F3">
-        <v>60.375</v>
+        <v>1.533525</v>
       </c>
       <c r="G3">
-        <v>67</v>
+        <v>1.7018</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -714,16 +714,16 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="K3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="L3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
       <c r="M3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +736,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:M3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,25 +829,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>12.5</v>
+        <v>0.3175</v>
       </c>
       <c r="B3">
-        <v>28.125</v>
+        <v>0.71437499999999998</v>
       </c>
       <c r="C3">
-        <v>40.5</v>
+        <v>1.0286999999999999</v>
       </c>
       <c r="D3">
-        <v>47.125</v>
+        <v>1.1969749999999999</v>
       </c>
       <c r="E3">
-        <v>53.75</v>
+        <v>1.3652499999999999</v>
       </c>
       <c r="F3">
-        <v>60.375</v>
+        <v>1.533525</v>
       </c>
       <c r="G3">
-        <v>67</v>
+        <v>1.7018</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -856,16 +856,16 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="K3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="L3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
       <c r="M3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
     </row>
   </sheetData>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8E3B4F-BAA0-4DA9-9879-36A731D2513A}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,25 +971,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>12.5</v>
+        <v>0.3175</v>
       </c>
       <c r="B3">
-        <v>28.125</v>
+        <v>0.71437499999999998</v>
       </c>
       <c r="C3">
-        <v>40.5</v>
+        <v>1.0286999999999999</v>
       </c>
       <c r="D3">
-        <v>47.125</v>
+        <v>1.1969749999999999</v>
       </c>
       <c r="E3">
-        <v>53.75</v>
+        <v>1.3652499999999999</v>
       </c>
       <c r="F3">
-        <v>60.375</v>
+        <v>1.533525</v>
       </c>
       <c r="G3">
-        <v>67</v>
+        <v>1.7018</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -998,16 +998,16 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="K3">
-        <v>37</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="L3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
       <c r="M3">
-        <v>52</v>
+        <v>1.3208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>